<commit_message>
Sepparate calculation block to with and without cp(mix)
</commit_message>
<xml_diff>
--- a/utils/chem_table.xlsx
+++ b/utils/chem_table.xlsx
@@ -2162,7 +2162,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2184,12 +2184,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2216,6 +2210,25 @@
       <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="7647"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="7647"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -2248,13 +2261,6 @@
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -2333,7 +2339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2357,93 +2363,85 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2451,44 +2449,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal_New Rev. 21.xls" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal_New TEELs Rev 20 &amp; 21" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2551,10 +2568,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2649,8 +2662,8 @@
   </sheetPr>
   <dimension ref="A1:BO252"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI112" activeCellId="0" sqref="AI112"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI120" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK131" activeCellId="0" sqref="AK131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5341,7 +5354,7 @@
       <c r="A21" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="7" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -5470,7 +5483,7 @@
       <c r="A22" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="7" t="s">
         <v>124</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -5767,7 +5780,7 @@
       </c>
       <c r="Y24" s="9"/>
       <c r="Z24" s="9"/>
-      <c r="AA24" s="17"/>
+      <c r="AA24" s="16"/>
       <c r="AB24" s="8" t="n">
         <v>104.9</v>
       </c>
@@ -6449,7 +6462,7 @@
       <c r="BA29" s="8" t="n">
         <v>0.151909</v>
       </c>
-      <c r="BB29" s="18" t="n">
+      <c r="BB29" s="17" t="n">
         <v>7.73E-005</v>
       </c>
       <c r="BC29" s="8" t="n">
@@ -8869,7 +8882,7 @@
       </c>
       <c r="Y49" s="9"/>
       <c r="Z49" s="9"/>
-      <c r="AA49" s="17"/>
+      <c r="AA49" s="16"/>
       <c r="AB49" s="8" t="n">
         <v>59.5</v>
       </c>
@@ -12207,7 +12220,7 @@
       <c r="A76" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B76" s="18" t="s">
         <v>234</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -13084,7 +13097,7 @@
       <c r="BL82" s="8"/>
       <c r="BM82" s="8"/>
       <c r="BN82" s="8"/>
-      <c r="BO82" s="20"/>
+      <c r="BO82" s="19"/>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
@@ -13383,7 +13396,7 @@
       </c>
       <c r="Y85" s="9"/>
       <c r="Z85" s="9"/>
-      <c r="AA85" s="17"/>
+      <c r="AA85" s="16"/>
       <c r="AB85" s="8" t="n">
         <v>7</v>
       </c>
@@ -14838,7 +14851,7 @@
       <c r="A97" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="7" t="s">
         <v>278</v>
       </c>
       <c r="C97" s="8" t="s">
@@ -15725,7 +15738,7 @@
       <c r="BL103" s="8"/>
       <c r="BM103" s="8"/>
       <c r="BN103" s="8"/>
-      <c r="BO103" s="21"/>
+      <c r="BO103" s="20"/>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="12" t="s">
@@ -18858,7 +18871,7 @@
       <c r="A129" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B129" s="19" t="s">
+      <c r="B129" s="18" t="s">
         <v>345</v>
       </c>
       <c r="C129" s="8" t="s">
@@ -19149,7 +19162,7 @@
       <c r="Z131" s="9" t="n">
         <v>925.8</v>
       </c>
-      <c r="AA131" s="17" t="n">
+      <c r="AA131" s="16" t="n">
         <v>1</v>
       </c>
       <c r="AB131" s="8" t="n">
@@ -19162,12 +19175,8 @@
       <c r="AG131" s="8"/>
       <c r="AH131" s="8"/>
       <c r="AI131" s="8"/>
-      <c r="AJ131" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK131" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ131" s="8"/>
+      <c r="AK131" s="8"/>
       <c r="AL131" s="8"/>
       <c r="AM131" s="8" t="n">
         <v>3</v>
@@ -19418,7 +19427,7 @@
       <c r="BO133" s="8"/>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="22" t="s">
+      <c r="A134" s="21" t="s">
         <v>352</v>
       </c>
       <c r="B134" s="8"/>
@@ -19466,7 +19475,7 @@
       <c r="Z134" s="9" t="n">
         <v>925.8</v>
       </c>
-      <c r="AA134" s="17" t="n">
+      <c r="AA134" s="16" t="n">
         <v>1</v>
       </c>
       <c r="AB134" s="8" t="n">
@@ -19592,7 +19601,7 @@
       <c r="Z135" s="9" t="n">
         <v>170.5</v>
       </c>
-      <c r="AA135" s="17" t="n">
+      <c r="AA135" s="16" t="n">
         <v>1.43</v>
       </c>
       <c r="AB135" s="8" t="n">
@@ -22335,7 +22344,7 @@
       <c r="BL156" s="8"/>
       <c r="BM156" s="8"/>
       <c r="BN156" s="8"/>
-      <c r="BO156" s="20"/>
+      <c r="BO156" s="19"/>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="6" t="s">
@@ -28473,7 +28482,7 @@
       </c>
       <c r="AR205" s="8"/>
       <c r="AS205" s="8"/>
-      <c r="AT205" s="21"/>
+      <c r="AT205" s="20"/>
       <c r="AU205" s="8"/>
       <c r="AV205" s="8" t="n">
         <v>0.843</v>
@@ -29715,7 +29724,7 @@
       <c r="BB216" s="8" t="n">
         <v>5.1E-005</v>
       </c>
-      <c r="BC216" s="23" t="n">
+      <c r="BC216" s="22" t="n">
         <f aca="false">IF(AND(Fract_Sulfuric&lt;1,Fract_Aq&gt;0),15.416-26*(1-Fract_Sulfuric),15.416)</f>
         <v>15.416</v>
       </c>
@@ -31607,7 +31616,7 @@
       <c r="BA232" s="8" t="n">
         <v>0.0375</v>
       </c>
-      <c r="BB232" s="18" t="n">
+      <c r="BB232" s="17" t="n">
         <v>6.3E-005</v>
       </c>
       <c r="BC232" s="8" t="n">
@@ -33324,7 +33333,7 @@
       </c>
       <c r="Y246" s="9"/>
       <c r="Z246" s="9"/>
-      <c r="AA246" s="17"/>
+      <c r="AA246" s="16"/>
       <c r="AB246" s="8" t="n">
         <v>72.8</v>
       </c>
@@ -33410,7 +33419,7 @@
       <c r="A247" s="6" t="s">
         <v>578</v>
       </c>
-      <c r="B247" s="24" t="s">
+      <c r="B247" s="23" t="s">
         <v>579</v>
       </c>
       <c r="C247" s="8" t="s">
@@ -33654,118 +33663,118 @@
       <c r="BN248" s="8"/>
       <c r="BO248" s="8"/>
     </row>
-    <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="6" t="s">
+    <row r="249" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B249" s="8" t="s">
+      <c r="B249" s="25" t="s">
         <v>582</v>
       </c>
-      <c r="C249" s="8" t="s">
+      <c r="C249" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D249" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E249" s="8"/>
-      <c r="F249" s="6" t="s">
+      <c r="D249" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E249" s="25"/>
+      <c r="F249" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="G249" s="8"/>
-      <c r="H249" s="8"/>
-      <c r="I249" s="8"/>
-      <c r="J249" s="8"/>
-      <c r="K249" s="8"/>
-      <c r="L249" s="8"/>
-      <c r="M249" s="8"/>
-      <c r="N249" s="8"/>
-      <c r="O249" s="8"/>
-      <c r="P249" s="8"/>
-      <c r="Q249" s="8"/>
-      <c r="R249" s="8"/>
-      <c r="S249" s="8"/>
-      <c r="T249" s="8" t="n">
+      <c r="G249" s="25"/>
+      <c r="H249" s="25"/>
+      <c r="I249" s="25"/>
+      <c r="J249" s="25"/>
+      <c r="K249" s="25"/>
+      <c r="L249" s="25"/>
+      <c r="M249" s="25"/>
+      <c r="N249" s="25"/>
+      <c r="O249" s="25"/>
+      <c r="P249" s="25"/>
+      <c r="Q249" s="25"/>
+      <c r="R249" s="25"/>
+      <c r="S249" s="25"/>
+      <c r="T249" s="25" t="n">
         <v>18.02</v>
       </c>
-      <c r="U249" s="8"/>
-      <c r="V249" s="8"/>
-      <c r="W249" s="8"/>
-      <c r="X249" s="8"/>
-      <c r="Y249" s="9"/>
-      <c r="Z249" s="9"/>
-      <c r="AA249" s="8"/>
-      <c r="AB249" s="8" t="n">
+      <c r="U249" s="25"/>
+      <c r="V249" s="25"/>
+      <c r="W249" s="25"/>
+      <c r="X249" s="25"/>
+      <c r="Y249" s="26"/>
+      <c r="Z249" s="26"/>
+      <c r="AA249" s="25"/>
+      <c r="AB249" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="AC249" s="8" t="n">
+      <c r="AC249" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="AD249" s="8"/>
-      <c r="AE249" s="8"/>
-      <c r="AF249" s="8"/>
-      <c r="AG249" s="8"/>
-      <c r="AH249" s="8"/>
-      <c r="AI249" s="8"/>
-      <c r="AJ249" s="8"/>
-      <c r="AK249" s="8"/>
-      <c r="AL249" s="8"/>
-      <c r="AM249" s="8" t="n">
+      <c r="AD249" s="25"/>
+      <c r="AE249" s="25"/>
+      <c r="AF249" s="25"/>
+      <c r="AG249" s="25"/>
+      <c r="AH249" s="25"/>
+      <c r="AI249" s="25"/>
+      <c r="AJ249" s="25"/>
+      <c r="AK249" s="25"/>
+      <c r="AL249" s="25"/>
+      <c r="AM249" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="AN249" s="8" t="n">
+      <c r="AN249" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="AO249" s="8" t="n">
+      <c r="AO249" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="AP249" s="8"/>
-      <c r="AQ249" s="8"/>
-      <c r="AR249" s="8"/>
-      <c r="AS249" s="8"/>
-      <c r="AT249" s="8"/>
-      <c r="AU249" s="8" t="s">
+      <c r="AP249" s="25"/>
+      <c r="AQ249" s="25"/>
+      <c r="AR249" s="25"/>
+      <c r="AS249" s="25"/>
+      <c r="AT249" s="25"/>
+      <c r="AU249" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AV249" s="8" t="n">
+      <c r="AV249" s="25" t="n">
         <v>1.017</v>
       </c>
-      <c r="AW249" s="8" t="n">
+      <c r="AW249" s="25" t="n">
         <v>0.00078</v>
       </c>
-      <c r="AX249" s="8" t="n">
+      <c r="AX249" s="25" t="n">
         <v>0.983</v>
       </c>
-      <c r="AY249" s="10" t="n">
+      <c r="AY249" s="27" t="n">
         <v>0.000567</v>
       </c>
-      <c r="AZ249" s="8" t="n">
+      <c r="AZ249" s="25" t="n">
         <v>596.3</v>
       </c>
-      <c r="BA249" s="8" t="n">
+      <c r="BA249" s="25" t="n">
         <v>0.455</v>
       </c>
-      <c r="BB249" s="8" t="n">
+      <c r="BB249" s="25" t="n">
         <v>0.001035</v>
       </c>
-      <c r="BC249" s="8" t="n">
+      <c r="BC249" s="25" t="n">
         <v>11.7124</v>
       </c>
-      <c r="BD249" s="8" t="n">
+      <c r="BD249" s="25" t="n">
         <v>3853.28</v>
       </c>
-      <c r="BE249" s="8" t="n">
+      <c r="BE249" s="25" t="n">
         <v>44.13</v>
       </c>
-      <c r="BF249" s="8"/>
-      <c r="BG249" s="8"/>
-      <c r="BH249" s="8"/>
-      <c r="BI249" s="8"/>
-      <c r="BJ249" s="8"/>
-      <c r="BK249" s="8"/>
-      <c r="BL249" s="8"/>
-      <c r="BM249" s="8"/>
-      <c r="BN249" s="8"/>
-      <c r="BO249" s="8"/>
+      <c r="BF249" s="25"/>
+      <c r="BG249" s="25"/>
+      <c r="BH249" s="25"/>
+      <c r="BI249" s="25"/>
+      <c r="BJ249" s="25"/>
+      <c r="BK249" s="25"/>
+      <c r="BL249" s="25"/>
+      <c r="BM249" s="25"/>
+      <c r="BN249" s="25"/>
+      <c r="BO249" s="25"/>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="14" t="s">
@@ -33861,7 +33870,7 @@
       <c r="BC250" s="8" t="n">
         <v>11.7124</v>
       </c>
-      <c r="BD250" s="23" t="n">
+      <c r="BD250" s="22" t="n">
         <f aca="false">IF(Chemical="Sulfuric Acid - 90% aqueous",5077.43,3853.28+EXP(7.9*Fract_Sulfuric^0.5)-1)</f>
         <v>3853.28</v>
       </c>
@@ -34007,129 +34016,129 @@
       <c r="BO251" s="8"/>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="25"/>
-      <c r="B252" s="25"/>
-      <c r="C252" s="26" t="s">
+      <c r="A252" s="29"/>
+      <c r="B252" s="29"/>
+      <c r="C252" s="30" t="s">
         <v>586</v>
       </c>
-      <c r="D252" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E252" s="26"/>
-      <c r="F252" s="26"/>
-      <c r="G252" s="26"/>
-      <c r="H252" s="26"/>
-      <c r="I252" s="26"/>
-      <c r="J252" s="26"/>
-      <c r="K252" s="26"/>
-      <c r="L252" s="26"/>
-      <c r="M252" s="26"/>
-      <c r="N252" s="26"/>
-      <c r="O252" s="26"/>
-      <c r="P252" s="26"/>
-      <c r="Q252" s="26"/>
-      <c r="R252" s="26"/>
-      <c r="S252" s="26"/>
-      <c r="T252" s="21" t="n">
+      <c r="D252" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E252" s="30"/>
+      <c r="F252" s="30"/>
+      <c r="G252" s="30"/>
+      <c r="H252" s="30"/>
+      <c r="I252" s="30"/>
+      <c r="J252" s="30"/>
+      <c r="K252" s="30"/>
+      <c r="L252" s="30"/>
+      <c r="M252" s="30"/>
+      <c r="N252" s="30"/>
+      <c r="O252" s="30"/>
+      <c r="P252" s="30"/>
+      <c r="Q252" s="30"/>
+      <c r="R252" s="30"/>
+      <c r="S252" s="30"/>
+      <c r="T252" s="20" t="n">
         <v>130.19</v>
       </c>
-      <c r="U252" s="21"/>
-      <c r="V252" s="21" t="n">
+      <c r="U252" s="20"/>
+      <c r="V252" s="20" t="n">
         <v>100</v>
       </c>
-      <c r="W252" s="21" t="n">
+      <c r="W252" s="20" t="n">
         <v>1000</v>
       </c>
-      <c r="X252" s="21"/>
-      <c r="Y252" s="21"/>
-      <c r="Z252" s="21"/>
-      <c r="AA252" s="21"/>
-      <c r="AB252" s="21" t="n">
+      <c r="X252" s="20"/>
+      <c r="Y252" s="20"/>
+      <c r="Z252" s="20"/>
+      <c r="AA252" s="20"/>
+      <c r="AB252" s="20" t="n">
         <v>149.3</v>
       </c>
-      <c r="AC252" s="21" t="n">
+      <c r="AC252" s="20" t="n">
         <v>-71</v>
       </c>
-      <c r="AD252" s="21"/>
-      <c r="AE252" s="21"/>
-      <c r="AF252" s="21"/>
-      <c r="AG252" s="21"/>
-      <c r="AH252" s="21"/>
-      <c r="AI252" s="21" t="n">
+      <c r="AD252" s="20"/>
+      <c r="AE252" s="20"/>
+      <c r="AF252" s="20"/>
+      <c r="AG252" s="20"/>
+      <c r="AH252" s="20"/>
+      <c r="AI252" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="AJ252" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK252" s="21"/>
-      <c r="AL252" s="21"/>
-      <c r="AM252" s="21" t="n">
+      <c r="AJ252" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK252" s="20"/>
+      <c r="AL252" s="20"/>
+      <c r="AM252" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="AN252" s="21" t="n">
+      <c r="AN252" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="AO252" s="21" t="n">
+      <c r="AO252" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AP252" s="21"/>
-      <c r="AQ252" s="21"/>
-      <c r="AR252" s="21"/>
-      <c r="AS252" s="21"/>
-      <c r="AT252" s="21"/>
-      <c r="AU252" s="21" t="s">
+      <c r="AP252" s="20"/>
+      <c r="AQ252" s="20"/>
+      <c r="AR252" s="20"/>
+      <c r="AS252" s="20"/>
+      <c r="AT252" s="20"/>
+      <c r="AU252" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="AV252" s="21" t="n">
+      <c r="AV252" s="20" t="n">
         <v>0.893</v>
       </c>
-      <c r="AW252" s="21" t="n">
+      <c r="AW252" s="20" t="n">
         <v>0.001046</v>
       </c>
-      <c r="AX252" s="21" t="n">
+      <c r="AX252" s="20" t="n">
         <v>0.439</v>
       </c>
-      <c r="AY252" s="27" t="n">
+      <c r="AY252" s="31" t="n">
         <v>0.0009417</v>
       </c>
-      <c r="AZ252" s="21" t="n">
+      <c r="AZ252" s="20" t="n">
         <v>92.7</v>
       </c>
-      <c r="BA252" s="21" t="n">
+      <c r="BA252" s="20" t="n">
         <v>0.118611</v>
       </c>
-      <c r="BB252" s="21" t="n">
+      <c r="BB252" s="20" t="n">
         <v>0.000181</v>
       </c>
-      <c r="BC252" s="21" t="n">
+      <c r="BC252" s="20" t="n">
         <v>10.5116</v>
       </c>
-      <c r="BD252" s="21" t="n">
+      <c r="BD252" s="20" t="n">
         <v>3932.03</v>
       </c>
-      <c r="BE252" s="21" t="n">
+      <c r="BE252" s="20" t="n">
         <v>49.59</v>
       </c>
-      <c r="BF252" s="21"/>
-      <c r="BG252" s="21" t="n">
+      <c r="BF252" s="20"/>
+      <c r="BG252" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="BH252" s="21" t="n">
+      <c r="BH252" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="BI252" s="21" t="n">
+      <c r="BI252" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="BJ252" s="21" t="n">
+      <c r="BJ252" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="BK252" s="21" t="n">
+      <c r="BK252" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="BL252" s="25"/>
-      <c r="BM252" s="21"/>
-      <c r="BN252" s="21"/>
-      <c r="BO252" s="21"/>
+      <c r="BL252" s="29"/>
+      <c r="BM252" s="20"/>
+      <c r="BN252" s="20"/>
+      <c r="BO252" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -34139,7 +34148,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>